<commit_message>
organizing results and data
</commit_message>
<xml_diff>
--- a/Data/2016/04_April/20160426_TN_reps_WWRQ45_done_on_20160408.xlsx
+++ b/Data/2016/04_April/20160426_TN_reps_WWRQ45_done_on_20160408.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2040" windowWidth="24780" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="20360" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -79,21 +82,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,7 +491,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
@@ -559,7 +591,7 @@
             <c:numRef>
               <c:f>Sheet1!$E$2:$E$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.976594499707431</c:v>
@@ -639,7 +671,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1055,7 +1087,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1084,11 +1116,11 @@
       <c r="C2">
         <v>0.76036446469248287</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>B2/MAX($B$2:$B$13)</f>
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <f>C2/MAX($C$2:$C$13)</f>
         <v>0.97659449970743117</v>
       </c>
@@ -1103,11 +1135,11 @@
       <c r="C3">
         <v>0.76947608200455575</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D13" si="0">B3/MAX($B$2:$B$13)</f>
         <v>0.9842188321935823</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E13" si="1">C3/MAX($C$2:$C$13)</f>
         <v>0.98829724985371548</v>
       </c>
@@ -1122,11 +1154,11 @@
       <c r="C4">
         <v>0.77858769931662875</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>0.97369805365597051</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1141,11 +1173,11 @@
       <c r="C5">
         <v>0.63963553530751704</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>0.79484481851657018</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <f t="shared" si="1"/>
         <v>0.82153306026916317</v>
       </c>
@@ -1160,11 +1192,11 @@
       <c r="C6">
         <v>0.516628701594533</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>0.78695423461336156</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <f t="shared" si="1"/>
         <v>0.6635459332943241</v>
       </c>
@@ -1179,11 +1211,11 @@
       <c r="C7">
         <v>0.43917995444191343</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>0.72645975802209373</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <f t="shared" si="1"/>
         <v>0.56407255705090698</v>
       </c>
@@ -1198,11 +1230,11 @@
       <c r="C8">
         <v>0.37312072892938497</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>0.6396633350867964</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <f t="shared" si="1"/>
         <v>0.47922761849034523</v>
       </c>
@@ -1217,11 +1249,11 @@
       <c r="C9">
         <v>0.36856492027334847</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>0.57390846922672278</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <f t="shared" si="1"/>
         <v>0.47337624341720297</v>
       </c>
@@ -1236,11 +1268,11 @@
       <c r="C10">
         <v>0.33667425968109344</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>0.48185165702261967</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <f t="shared" si="1"/>
         <v>0.43241661790520775</v>
       </c>
@@ -1255,11 +1287,11 @@
       <c r="C11">
         <v>0.27289293849658314</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>0.37927406628090476</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <f t="shared" si="1"/>
         <v>0.35049736688121708</v>
       </c>
@@ -1274,11 +1306,11 @@
       <c r="C12">
         <v>0.24555808656036443</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>0.38716465018411361</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f t="shared" si="1"/>
         <v>0.31538911644236389</v>
       </c>
@@ -1293,11 +1325,11 @@
       <c r="C13">
         <v>0.23644646924829155</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <f t="shared" si="0"/>
         <v>0.39242503945291957</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f t="shared" si="1"/>
         <v>0.30368636629607954</v>
       </c>

</xml_diff>